<commit_message>
0804 changing it back to no simple case
</commit_message>
<xml_diff>
--- a/results/excel/0725-n15.xlsx
+++ b/results/excel/0725-n15.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b0190\Dropbox\USC\publication\gcn\smuggler_networks\results\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2768785F-ADC7-4104-8CD4-D09815EEF0D2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2E7CE1-77E0-46D3-8D4C-B9A738B09002}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7866,6 +7866,3666 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.22447562236538618"/>
+          <c:y val="6.8209310227658845E-2"/>
+          <c:w val="0.72261544579654813"/>
+          <c:h val="0.66601068675974495"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>two-stage</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'2S-global'!$H$1:$BE$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>49</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'2S-global'!$H$4:$BE$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>1.2608938504</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1838108489999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.63821688720000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.42073901060000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.35090119060000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.31481100779999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.28529745400000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.2603826326</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.23004383599999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.198210889</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.16635879479999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.13609638460000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.11249971839999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.1014107152</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.4009642200000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.0670688999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.815178139999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.3315568800000017E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.0980256200000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.6832655200000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.7029770400000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7.3584873000000009E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7.1485951999999992E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6.9942733199999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6.8507720000000008E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.8300168600000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.7044829599999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6.6956029399999992E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6.7202094000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6.6446103399999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3092-456A-A278-739B316A7415}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1379660320"/>
+        <c:axId val="1694989728"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:v>full-DF</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="triangle"/>
+                  <c:size val="7"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'DF-global'!$H$1:$BE$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="50"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>26</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>28</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>29</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>31</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>34</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>35</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>36</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>37</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>38</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>39</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>41</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>42</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>43</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>44</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>45</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>46</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>47</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>48</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>49</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'DF-global'!$H$4:$BE$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="50"/>
+                      <c:pt idx="0">
+                        <c:v>1.2608938504</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.2266783083999999</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.93970849519999999</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.8109792172000001</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.62768735340000004</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.52842482800000001</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.43932167519999998</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.30078312639999999</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.26339910799999999</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.24647799079999996</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.25016148039999997</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.22201036460000001</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.2329498552</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.22953203279999998</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.2286601644</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>0.22846559859999999</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0.22686813780000001</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>0.22993981620000001</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>0.22970096719999997</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>0.2281935444</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>0.22897752360000001</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>0.2280578566</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>0.22832788079999999</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>0.22784292059999997</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>0.22790324980000004</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>0.22788525139999999</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>0.22803184160000001</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>0.22805252100000004</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>0.2280726076</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>0.22798876520000003</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="1"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-3092-456A-A278-739B316A7415}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:v>fast-DF</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="square"/>
+                  <c:size val="7"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'DF-mincut'!$H$1:$BE$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="50"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>26</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>28</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>29</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>31</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>34</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>35</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>36</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>37</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>38</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>39</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>41</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>42</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>43</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>44</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>45</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>46</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>47</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>48</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>49</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'DF-mincut'!$H$4:$BE$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="50"/>
+                      <c:pt idx="0">
+                        <c:v>1.2608938504</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.2174355113999999</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.90296576379999993</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.72980799480000003</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.66472326559999995</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.61157286319999993</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.56352775939999999</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.53302829500000004</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.50611358440000009</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.46829380100000001</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.46623540600000002</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.43974403439999998</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.42798417919999998</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.42467132800000007</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.42359666579999999</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>0.42372197319999999</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0.42095471699999998</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>0.42017443779999997</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>0.42051370919999992</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>0.41745735519999999</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>0.41913035140000005</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>0.41709346859999996</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>0.41650071980000003</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>0.41595459940000001</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>0.41591029339999996</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>0.41583292979999997</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>0.41565221819999998</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>0.41580987320000001</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>0.41564247759999995</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>0.41551696180000003</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="1"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-3092-456A-A278-739B316A7415}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:v>fast-2S</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="diamond"/>
+                  <c:size val="7"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'2S-mincut'!$H$1:$BE$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="50"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>26</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>28</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>29</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>31</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>34</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>35</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>36</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>37</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>38</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>39</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>41</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>42</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>43</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>44</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>45</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>46</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>47</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>48</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>49</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'2S-mincut'!$H$4:$BE$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="50"/>
+                      <c:pt idx="0">
+                        <c:v>1.2608938504</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.1838108489999999</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.63821688720000003</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.42073901060000002</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.35090119060000002</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.31481100779999999</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.28529745400000001</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.2603826326</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.23004383599999997</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.198210889</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.16635879479999999</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.13609638460000001</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.11249971839999999</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.1014107152</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>9.4009642200000007E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>9.0670688999999999E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>8.815178139999999E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>8.3315568800000017E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>8.0980256200000003E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>7.6832655200000002E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>7.7029770400000003E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>7.3584873000000009E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>7.1485951999999992E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>6.9942733199999996E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>6.8507720000000008E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>6.8300168600000002E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>6.7044829599999994E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>6.6956029399999992E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>6.7202094000000004E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>6.6446103399999998E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="1"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-3092-456A-A278-739B316A7415}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1379660320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="25"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>epochs</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" sz="1800">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1694989728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="5"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1694989728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.4"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>KL-divergence</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" sz="1800">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1379660320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.48399027137736822"/>
+          <c:y val="8.824881073734285E-2"/>
+          <c:w val="0.43472452636968767"/>
+          <c:h val="0.25639058783554197"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr b="1"/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-TW"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0" l="0" r="0" t="0" header="0.31496062992125984" footer="0.31496062992125984"/>
+    <c:pageSetup paperSize="5" orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.24411361629660736"/>
+          <c:y val="8.4193000339789326E-2"/>
+          <c:w val="0.70080770318596974"/>
+          <c:h val="0.65424814827940603"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>two-stage</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'2S-global'!$H$7:$BE$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>49</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'2S-global'!$H$10:$BE$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>-3.3482192518000007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3.3177905274000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.1057215715999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3.1218586899999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-3.0857919550000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-3.0796362924000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-3.0418915296</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-3.0376184727999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-3.0182191632000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-2.9710096809999995</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-2.9628098132000003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-2.9652406785999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-2.9678648020000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2.9936991237999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-3.0075073457999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-3.0181655766</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-3.0383991907999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-3.0112622115999996</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-3.0320384262000006</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-3.010929768</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-3.0088344076000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-3.0205621575999997</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-3.015897286</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-3.0104172849999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-3.0212022948000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-3.0414948798000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-3.0319908884000002</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-3.0282021618000003</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-3.0391755749999998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-3.0256596780000002</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3988-46A7-AE79-8CED95B14EDB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1379660320"/>
+        <c:axId val="1694989728"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:v>full-DF</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="triangle"/>
+                  <c:size val="7"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'DF-global'!$H$7:$BE$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="50"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>26</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>28</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>29</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>31</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>34</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>35</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>36</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>37</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>38</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>39</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>41</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>42</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>43</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>44</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>45</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>46</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>47</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>48</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>49</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'DF-global'!$H$10:$BE$10</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="50"/>
+                      <c:pt idx="0">
+                        <c:v>-3.3482192518000007</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>-3.3291656258000004</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>-3.1419010997999997</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>-3.0802788780000006</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>-3.0186343193999998</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>-3.1759796738000001</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>-2.9771228409999999</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>-2.9142310428</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>-2.8309451748000001</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>-2.8299801969999998</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>-2.8252913546</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>-2.79794842</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>-2.7873201035999999</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>-2.7962137605999997</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>-2.7878438831999999</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>-2.7819207881999999</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>-2.7783709599999997</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>-2.7912845561999999</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>-2.7876730633999998</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>-2.7862663909999994</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>-2.7858563278000004</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>-2.7856552816</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>-2.7855587362000001</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>-2.7853794122000002</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>-2.7853387118000001</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>-2.7852709818000001</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>-2.7854295514</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>-2.7853480743999999</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>-2.7853444313999995</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>-2.7853076840000002</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="1"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-3988-46A7-AE79-8CED95B14EDB}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:v>fast-DF</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="square"/>
+                  <c:size val="7"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'DF-mincut'!$H$7:$BE$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="50"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>26</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>28</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>29</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>31</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>34</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>35</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>36</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>37</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>38</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>39</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>41</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>42</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>43</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>44</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>45</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>46</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>47</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>48</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>49</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'DF-mincut'!$H$10:$BE$10</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="50"/>
+                      <c:pt idx="0">
+                        <c:v>-3.4507560491999998</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>-3.4126772214000001</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>-3.1034766698</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>-3.0145853330000003</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>-2.9783738972</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>-2.9569593738000002</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>-2.9327616929999998</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>-2.9097122238000002</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>-2.8945117806000003</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>-2.8883346603999995</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>-2.8849441647999998</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>-2.8792577671999999</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>-2.8739632272</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>-2.8748287319999997</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>-2.8751236485999998</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>-2.8749219681999998</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>-2.8745377779999997</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>-2.8743356419999997</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>-2.8738996337999998</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>-2.8747650001999996</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>-2.8742624327999997</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>-2.874053719</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>-2.8739417863999996</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>-2.8742656947999996</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>-2.8741948005999998</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>-2.8742654418</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>-2.8745140527999995</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>-2.8742630862</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>-2.8742680190000001</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>-2.8761992333999999</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="1"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-3988-46A7-AE79-8CED95B14EDB}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:v>fast-2S</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="diamond"/>
+                  <c:size val="7"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'2S-mincut'!$H$7:$BE$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="50"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>26</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>28</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>29</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>31</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>34</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>35</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>36</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>37</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>38</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>39</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>41</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>42</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>43</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>44</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>45</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>46</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>47</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>48</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>49</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'2S-mincut'!$H$10:$BE$10</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="50"/>
+                      <c:pt idx="0">
+                        <c:v>-3.4507560491999998</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>-3.4034058238</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>-3.0275172304</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>-3.1487536644</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>-3.0957875917999997</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>-3.0925384712000001</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>-3.0549959159999998</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>-3.0446579408000001</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>-3.0258163260000002</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>-3.0038151504000004</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>-3.0134851143999999</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>-3.0235812186</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>-3.0310135032000001</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>-3.0496516562</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>-3.0579415796</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>-3.0601900148000003</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>-3.0771695424000001</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>-3.0565194822000001</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>-3.0660372067999999</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>-3.0623341799999997</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>-3.0655690836000002</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>-3.0673708250000002</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>-3.0657604624000001</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>-3.0641312956000002</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>-3.0527474257999998</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>-3.0774977112000004</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>-3.0644141888000003</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>-3.0687489032000004</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>-3.0713068603999996</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>-3.0615178776</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="1"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-3988-46A7-AE79-8CED95B14EDB}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1379660320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="20"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>epochs</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1694989728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="5"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1694989728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="-2.9"/>
+          <c:min val="-3.4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>defender utility</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1379660320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.31859907834101381"/>
+          <c:y val="0.51008792048929663"/>
+          <c:w val="0.67164669738863292"/>
+          <c:h val="0.26875169894665313"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800" b="1"/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-TW"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0" l="0" r="0" t="0" header="0.31496062992125984" footer="0.31496062992125984"/>
+    <c:pageSetup paperSize="5" orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -7987,6 +11647,86 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -10090,6 +13830,1038 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -10239,6 +15011,82 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="圖表 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD4E225D-7189-4CD4-928E-AFDF7F80E86B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>190499</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>144599</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="圖表 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{354EFF70-16D2-48F3-A045-910276012D73}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -10546,8 +15394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BE470"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="J7" workbookViewId="0">
+      <selection activeCell="Y29" sqref="Y29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>

</xml_diff>